<commit_message>
fix: Fixed tests excel patient #268
</commit_message>
<xml_diff>
--- a/tests/excel_test/Pacientes.xlsx
+++ b/tests/excel_test/Pacientes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmart\Universidad\4\ISPP\Proyecto\Recursos\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11A31D4B-ECCC-4FE3-8396-1B36B118B734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51DFB2A5-9DCB-4948-A7E7-5F7AD84DEDDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -102,7 +102,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{48A65D9C-382F-4C05-9CFE-CD03D4B0B33C}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{A17C842F-B910-47F0-9F28-B49E78B14CF6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Puede tener el valor "X" para marcar que esta rehabilitado, si se deja vacio se guardara como no rehabilitado</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{48A65D9C-382F-4C05-9CFE-CD03D4B0B33C}">
       <text>
         <r>
           <rPr>
@@ -116,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{724CE420-185E-4E40-85D9-386F09AFA473}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{724CE420-185E-4E40-85D9-386F09AFA473}">
       <text>
         <r>
           <rPr>
@@ -136,7 +150,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>nombre</t>
   </si>
@@ -168,34 +182,52 @@
     <t>martin</t>
   </si>
   <si>
+    <t>Hombre</t>
+  </si>
+  <si>
+    <t>adsfkajdf</t>
+  </si>
+  <si>
+    <t>segundo apellido</t>
+  </si>
+  <si>
+    <t>primer apellido</t>
+  </si>
+  <si>
+    <t>jose maria</t>
+  </si>
+  <si>
+    <t>99186787T</t>
+  </si>
+  <si>
+    <t>joaquin</t>
+  </si>
+  <si>
+    <t>san marques</t>
+  </si>
+  <si>
+    <t>asdf</t>
+  </si>
+  <si>
+    <t>rehabilitado</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>maria</t>
+  </si>
+  <si>
     <t>cabrera</t>
   </si>
   <si>
-    <t>pepe</t>
-  </si>
-  <si>
-    <t>Hombre</t>
-  </si>
-  <si>
-    <t>San Bernardo</t>
-  </si>
-  <si>
-    <t>adsfkajdf</t>
-  </si>
-  <si>
-    <t>segundo apellido</t>
-  </si>
-  <si>
-    <t>primer apellido</t>
-  </si>
-  <si>
-    <t>29556849D</t>
-  </si>
-  <si>
-    <t>jose maria</t>
-  </si>
-  <si>
-    <t>iba borracho</t>
+    <t>65963475G</t>
+  </si>
+  <si>
+    <t>Mujer</t>
+  </si>
+  <si>
+    <t>nada</t>
   </si>
 </sst>
 </file>
@@ -253,26 +285,26 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
+  <dxfs count="13">
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2"/>
         </patternFill>
@@ -312,6 +344,14 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <fgColor indexed="64"/>
@@ -365,9 +405,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CEB08CD-B2E3-4683-96AE-3CFC301306B5}" name="Tabla1" displayName="Tabla1" ref="A1:K3" totalsRowShown="0" dataDxfId="0">
-  <autoFilter ref="A1:K3" xr:uid="{3CEB08CD-B2E3-4683-96AE-3CFC301306B5}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CEB08CD-B2E3-4683-96AE-3CFC301306B5}" name="Tabla1" displayName="Tabla1" ref="A1:L3" totalsRowShown="0" dataDxfId="12">
+  <autoFilter ref="A1:L3" xr:uid="{3CEB08CD-B2E3-4683-96AE-3CFC301306B5}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{2C2A0CF3-C8E8-4A82-80B8-E59F37D30B3C}" name="nombre" dataDxfId="11"/>
     <tableColumn id="2" xr3:uid="{990ADAC8-E7F4-406E-98F1-40C96776051C}" name="primer apellido" dataDxfId="10"/>
     <tableColumn id="3" xr3:uid="{1F836F1E-70F1-49AB-A637-8BDE5CEB4AC1}" name="segundo apellido" dataDxfId="9"/>
@@ -377,8 +417,9 @@
     <tableColumn id="7" xr3:uid="{F0B2A95A-FDB4-4EA5-9940-7595208E72F5}" name="direccion" dataDxfId="5"/>
     <tableColumn id="8" xr3:uid="{F540188F-4CDB-4E57-8B32-0E44AC357EA0}" name="telefono" dataDxfId="4"/>
     <tableColumn id="9" xr3:uid="{2D759B19-2887-4C55-B57B-7887AA48AA3A}" name="numero expediente" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{6F481A90-31E5-4A89-8EB6-19E8F09208B7}" name="tecnico" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{D2F6F8FD-B4CA-4E86-A23A-1BCF1C1C1037}" name="observacion" dataDxfId="1"/>
+    <tableColumn id="12" xr3:uid="{5AF19D54-0AF7-45C8-BE41-D6CAAE01B7D2}" name="rehabilitado" dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{6F481A90-31E5-4A89-8EB6-19E8F09208B7}" name="tecnico" dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{D2F6F8FD-B4CA-4E86-A23A-1BCF1C1C1037}" name="observacion" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -647,10 +688,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -658,25 +699,26 @@
     <col min="1" max="1" width="9.453125" customWidth="1"/>
     <col min="2" max="2" width="16.08984375" customWidth="1"/>
     <col min="3" max="3" width="17.26953125" customWidth="1"/>
-    <col min="4" max="4" width="9.7265625" customWidth="1"/>
+    <col min="4" max="4" width="5.54296875" customWidth="1"/>
     <col min="5" max="5" width="17.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.54296875" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" customWidth="1"/>
     <col min="9" max="9" width="19.7265625" customWidth="1"/>
-    <col min="10" max="10" width="9.81640625" customWidth="1"/>
-    <col min="11" max="11" width="13.453125" customWidth="1"/>
+    <col min="10" max="10" width="13.6328125" customWidth="1"/>
+    <col min="11" max="11" width="9.26953125" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -697,59 +739,80 @@
         <v>6</v>
       </c>
       <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
         <v>7</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E2" s="3">
         <v>36058</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="H2" s="2">
         <v>666666</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="3">
+        <v>36170</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
+      <c r="K3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>